<commit_message>
WIP on xml templating
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="131">
   <si>
     <t xml:space="preserve">Title</t>
   </si>
@@ -41,16 +41,40 @@
     <t xml:space="preserve">On going</t>
   </si>
   <si>
-    <t xml:space="preserve">Principal Investigator     (Fullname; email; organization)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Angelo Lupi; a.lupi@isac.cnr.it; ISP-CNR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Other Point of contacts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Mauro Mazzola; m.mazzola@isac.cnr.it: ISP-CNR</t>
+    <t xml:space="preserve">Principal Investigator fullname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Angelo Lupi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Investigator email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">a.lupi@isac.cnr.it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Principal Investigator organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISP-CNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point of contact fullname</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mauro Mazzola</t>
+  </si>
+  <si>
+    <t xml:space="preserve">←-- Leave empty if none</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point of contact email</t>
+  </si>
+  <si>
+    <t xml:space="preserve">m.mazzola@isac.cnr.it</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Point of contact organization</t>
   </si>
   <si>
     <t xml:space="preserve">Project Begin date (YYYY-MM-DD)</t>
@@ -59,7 +83,7 @@
     <t xml:space="preserve">Project End date (YYYY-MM-DD)</t>
   </si>
   <si>
-    <t xml:space="preserve">---</t>
+    <t xml:space="preserve">← Leave empty if no date</t>
   </si>
   <si>
     <t xml:space="preserve">Topic category</t>
@@ -400,7 +424,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -431,13 +455,6 @@
     </font>
     <font>
       <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -532,7 +549,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -565,12 +582,16 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -593,7 +614,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -674,17 +695,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D34"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="73.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="49.05"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="31.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -739,8 +760,8 @@
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
     </row>
-    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="3" t="s">
+    <row r="7" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -749,202 +770,224 @@
       <c r="C7" s="1"/>
       <c r="D7" s="2"/>
     </row>
-    <row r="8" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
+    <row r="8" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>11</v>
+      </c>
       <c r="C8" s="1"/>
       <c r="D8" s="2"/>
     </row>
-    <row r="9" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9" s="10" t="n">
-        <v>39073</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>12</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D9" s="2"/>
     </row>
-    <row r="10" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" customFormat="false" ht="31.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B11" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="2"/>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="1"/>
+      <c r="C11" s="1" t="s">
+        <v>14</v>
+      </c>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="11" t="s">
-        <v>14</v>
-      </c>
+    <row r="12" customFormat="false" ht="17.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="1"/>
       <c r="D12" s="2"/>
     </row>
     <row r="13" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>16</v>
+        <v>18</v>
+      </c>
+      <c r="B13" s="11" t="n">
+        <v>39073</v>
       </c>
       <c r="C13" s="1"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B14" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="1"/>
+        <v>19</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="1" t="s">
+        <v>20</v>
+      </c>
       <c r="D14" s="2"/>
     </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="12"/>
-      <c r="B15" s="13"/>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B16" s="14" t="s">
-        <v>20</v>
+        <v>21</v>
+      </c>
+      <c r="B16" s="12" t="s">
+        <v>22</v>
       </c>
       <c r="C16" s="1"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="12"/>
-      <c r="B17" s="13"/>
+    <row r="17" customFormat="false" ht="24.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>24</v>
+      </c>
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B18" s="11" t="s">
-        <v>22</v>
+        <v>25</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>26</v>
       </c>
       <c r="C18" s="1"/>
       <c r="D18" s="2"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A19" s="13"/>
+      <c r="B19" s="14"/>
       <c r="C19" s="1"/>
       <c r="D19" s="2"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="12"/>
-      <c r="B20" s="13"/>
+      <c r="A20" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20" s="15" t="s">
+        <v>28</v>
+      </c>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
     </row>
-    <row r="21" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B21" s="14" t="s">
-        <v>26</v>
-      </c>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="13"/>
+      <c r="B21" s="14"/>
       <c r="C21" s="1"/>
       <c r="D21" s="2"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="12"/>
-      <c r="B22" s="13"/>
+      <c r="A22" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>30</v>
+      </c>
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="B23" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>32</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="2"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="12"/>
-      <c r="B24" s="13"/>
+      <c r="A24" s="13"/>
+      <c r="B24" s="14"/>
       <c r="C24" s="1"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="22.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B25" s="14" t="s">
-        <v>30</v>
+        <v>33</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>34</v>
       </c>
       <c r="C25" s="1"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="13"/>
+      <c r="B26" s="14"/>
       <c r="C26" s="1"/>
       <c r="D26" s="2"/>
     </row>
-    <row r="27" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B27" s="14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C27" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C27" s="1"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="13"/>
+      <c r="B28" s="14"/>
       <c r="C28" s="1"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="2"/>
+    <row r="29" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="C29" s="1"/>
       <c r="D29" s="2"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="2"/>
+      <c r="C30" s="1"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
+    <row r="31" customFormat="false" ht="23.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="15" t="s">
+        <v>40</v>
+      </c>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="2"/>
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
       <c r="D32" s="2"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -959,25 +1002,49 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:B1"/>
-    <mergeCell ref="A28:C28"/>
+    <mergeCell ref="A32:C32"/>
   </mergeCells>
   <dataValidations count="4">
     <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B4" type="list">
       <formula1>Foglio2!$A$2:$A$19</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B13" type="list">
+    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B17" type="list">
       <formula1>Foglio2!$G$2:$G$35</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B21" type="list">
+    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B25" type="list">
       <formula1>Foglio2!$E$2:$E$21</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B12" type="list">
+    <dataValidation allowBlank="true" error="Clicca sulla freccia a destra della cella e scegli un valore dalla lista" errorTitle="Attenzione" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="B16" type="list">
       <formula1>Foglio2!$C$2:$C$22</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -1003,7 +1070,7 @@
       <selection pane="topLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.92"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="33.21"/>
@@ -1014,118 +1081,118 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="E1" s="15" t="s">
-        <v>33</v>
-      </c>
-      <c r="G1" s="15" t="s">
-        <v>15</v>
+      <c r="C1" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>41</v>
+      </c>
+      <c r="G1" s="16" t="s">
+        <v>23</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>44</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>51</v>
+        <v>59</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>52</v>
+        <v>60</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>53</v>
+        <v>61</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>54</v>
+        <v>62</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>55</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>56</v>
+        <v>64</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>59</v>
+        <v>67</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1133,248 +1200,248 @@
         <v>5</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>60</v>
+        <v>68</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>63</v>
+        <v>71</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>69</v>
+        <v>77</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>57</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>70</v>
+        <v>78</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>71</v>
+        <v>79</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>74</v>
+        <v>82</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>75</v>
+        <v>83</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>76</v>
+        <v>84</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>77</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>78</v>
+        <v>86</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>79</v>
+        <v>87</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>80</v>
+        <v>88</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>81</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>82</v>
+        <v>90</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>83</v>
+        <v>91</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>84</v>
+        <v>92</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>85</v>
+        <v>93</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>87</v>
+        <v>95</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>88</v>
+        <v>96</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>89</v>
+        <v>97</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>90</v>
+        <v>98</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>91</v>
+        <v>99</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>92</v>
+        <v>100</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>93</v>
+        <v>101</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>94</v>
+        <v>102</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>95</v>
+        <v>103</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>96</v>
+        <v>104</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>99</v>
+        <v>107</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>100</v>
+        <v>108</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>101</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C20" s="0" t="s">
-        <v>102</v>
+        <v>110</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>103</v>
+        <v>111</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>104</v>
+        <v>112</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C21" s="0" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C22" s="0" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>109</v>
+        <v>117</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G23" s="0" t="s">
-        <v>110</v>
+        <v>118</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G24" s="0" t="s">
-        <v>111</v>
+        <v>119</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G25" s="0" t="s">
-        <v>112</v>
+        <v>120</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G26" s="0" t="s">
-        <v>113</v>
+        <v>121</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G27" s="0" t="s">
-        <v>114</v>
+        <v>122</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G28" s="0" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G29" s="0" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G30" s="0" t="s">
-        <v>117</v>
+        <v>125</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G31" s="0" t="s">
-        <v>118</v>
+        <v>126</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G32" s="0" t="s">
-        <v>119</v>
+        <v>127</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G33" s="0" t="s">
-        <v>120</v>
+        <v>128</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G34" s="0" t="s">
-        <v>121</v>
+        <v>129</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="G35" s="0" t="s">
-        <v>122</v>
+        <v>130</v>
       </c>
     </row>
   </sheetData>

</xml_diff>